<commit_message>
Solve a predifined symetric tree
</commit_message>
<xml_diff>
--- a/Instances/01_NonStationary_b2_fe25_en_rk50_ll0_l20_HFalse_c2.xlsx
+++ b/Instances/01_NonStationary_b2_fe25_en_rk50_ll0_l20_HFalse_c2.xlsx
@@ -1467,7 +1467,7 @@
         <v>0.026</v>
       </c>
       <c r="E2" t="n">
-        <v>8.767200000000001</v>
+        <v>8.954400000000001</v>
       </c>
       <c r="F2" t="n">
         <v>0.052</v>
@@ -1499,7 +1499,7 @@
         <v>0.0248</v>
       </c>
       <c r="E3" t="n">
-        <v>2.1312</v>
+        <v>2.16</v>
       </c>
       <c r="F3" t="n">
         <v>0.04960000000000001</v>
@@ -1525,13 +1525,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="D4" t="n">
         <v>0.0048</v>
       </c>
       <c r="E4" t="n">
-        <v>3.408</v>
+        <v>3.475200000000001</v>
       </c>
       <c r="F4" t="n">
         <v>0.009600000000000001</v>
@@ -1557,13 +1557,13 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="D5" t="n">
         <v>0.002</v>
       </c>
       <c r="E5" t="n">
-        <v>1.42</v>
+        <v>1.448</v>
       </c>
       <c r="F5" t="n">
         <v>0.004</v>
@@ -1589,13 +1589,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="D6" t="n">
         <v>0.0036</v>
       </c>
       <c r="E6" t="n">
-        <v>2.556</v>
+        <v>2.6064</v>
       </c>
       <c r="F6" t="n">
         <v>0.007200000000000001</v>
@@ -1621,7 +1621,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>489</v>
+        <v>513</v>
       </c>
       <c r="D7" t="n">
         <v>0.026</v>
@@ -1653,7 +1653,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D8" t="n">
         <v>0.026</v>
@@ -1685,7 +1685,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D9" t="n">
         <v>0.0248</v>
@@ -1774,13 +1774,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="H2" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" t="n">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1803,13 +1803,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>221</v>
+        <v>249</v>
       </c>
       <c r="H3" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1835,10 +1835,10 @@
         <v>236</v>
       </c>
       <c r="H4" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" t="n">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1861,13 +1861,13 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="H5" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I5" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1935,13 +1935,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>33.5</v>
+        <v>33</v>
       </c>
       <c r="H2" t="n">
-        <v>5.625</v>
+        <v>5.5</v>
       </c>
       <c r="I2" t="n">
-        <v>8.875</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1964,13 +1964,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>41.4375</v>
+        <v>46.6875</v>
       </c>
       <c r="H3" t="n">
-        <v>8.4375</v>
+        <v>8.25</v>
       </c>
       <c r="I3" t="n">
-        <v>13.875</v>
+        <v>13.6875</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1996,10 +1996,10 @@
         <v>51.625</v>
       </c>
       <c r="H4" t="n">
-        <v>9.84375</v>
+        <v>9.625</v>
       </c>
       <c r="I4" t="n">
-        <v>15.96875</v>
+        <v>16.40625</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2022,13 +2022,13 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>50.859375</v>
+        <v>51.328125</v>
       </c>
       <c r="H5" t="n">
-        <v>10.546875</v>
+        <v>10.78125</v>
       </c>
       <c r="I5" t="n">
-        <v>17.578125</v>
+        <v>17.34375</v>
       </c>
     </row>
   </sheetData>
@@ -2068,7 +2068,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>7100</v>
+        <v>7240</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2076,7 +2076,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>37630</v>
+        <v>38372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>